<commit_message>
all bugs are removed
</commit_message>
<xml_diff>
--- a/doc/TLE.xlsx
+++ b/doc/TLE.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="65">
   <si>
     <t>T</t>
     <phoneticPr fontId="1"/>
@@ -804,6 +804,10 @@
     <t>TLE</t>
     <phoneticPr fontId="1"/>
   </si>
+  <si>
+    <t>-</t>
+    <phoneticPr fontId="1"/>
+  </si>
 </sst>
 </file>
 
@@ -1244,6 +1248,24 @@
     <xf numFmtId="0" fontId="6" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1256,9 +1278,6 @@
     <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1267,21 +1286,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2873,7 +2877,7 @@
   <dimension ref="A1:BW38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E34" sqref="E34"/>
+      <selection activeCell="AF19" sqref="AF19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.625" defaultRowHeight="12.75" x14ac:dyDescent="0.15"/>
@@ -3469,7 +3473,7 @@
         <v>20</v>
       </c>
       <c r="BH4" s="12" t="s">
-        <v>19</v>
+        <v>2</v>
       </c>
       <c r="BI4" s="12" t="s">
         <v>19</v>
@@ -4276,13 +4280,13 @@
       <c r="BW10" s="32"/>
     </row>
     <row r="11" spans="1:75" x14ac:dyDescent="0.15">
-      <c r="A11" s="46" t="s">
+      <c r="A11" s="52" t="s">
         <v>62</v>
       </c>
-      <c r="B11" s="47"/>
-      <c r="C11" s="47"/>
-      <c r="D11" s="47"/>
-      <c r="E11" s="47"/>
+      <c r="B11" s="53"/>
+      <c r="C11" s="53"/>
+      <c r="D11" s="53"/>
+      <c r="E11" s="53"/>
       <c r="F11" s="25"/>
       <c r="G11" s="25"/>
       <c r="H11" s="25"/>
@@ -4892,7 +4896,7 @@
         <v>20</v>
       </c>
       <c r="BH15" s="15" t="s">
-        <v>19</v>
+        <v>64</v>
       </c>
       <c r="BI15" s="15" t="s">
         <v>19</v>
@@ -5022,22 +5026,22 @@
       <c r="R17" s="33"/>
       <c r="S17" s="33"/>
       <c r="T17" s="33"/>
-      <c r="U17" s="57" t="s">
+      <c r="U17" s="50" t="s">
         <v>46</v>
       </c>
-      <c r="V17" s="57"/>
-      <c r="W17" s="57"/>
-      <c r="X17" s="57"/>
-      <c r="Y17" s="57"/>
-      <c r="Z17" s="57"/>
-      <c r="AA17" s="57"/>
-      <c r="AB17" s="57"/>
-      <c r="AC17" s="57"/>
-      <c r="AD17" s="57"/>
-      <c r="AE17" s="57"/>
-      <c r="AF17" s="57"/>
-      <c r="AG17" s="57"/>
-      <c r="AH17" s="57"/>
+      <c r="V17" s="50"/>
+      <c r="W17" s="50"/>
+      <c r="X17" s="50"/>
+      <c r="Y17" s="50"/>
+      <c r="Z17" s="50"/>
+      <c r="AA17" s="50"/>
+      <c r="AB17" s="50"/>
+      <c r="AC17" s="50"/>
+      <c r="AD17" s="50"/>
+      <c r="AE17" s="50"/>
+      <c r="AF17" s="50"/>
+      <c r="AG17" s="50"/>
+      <c r="AH17" s="50"/>
       <c r="AI17" s="33"/>
       <c r="AJ17" s="33"/>
       <c r="AK17" s="33"/>
@@ -5072,14 +5076,14 @@
       <c r="BN17" s="33"/>
       <c r="BO17" s="33"/>
       <c r="BP17" s="33"/>
-      <c r="BQ17" s="57" t="s">
+      <c r="BQ17" s="50" t="s">
         <v>40</v>
       </c>
-      <c r="BR17" s="57"/>
-      <c r="BS17" s="57"/>
-      <c r="BT17" s="57"/>
-      <c r="BU17" s="57"/>
-      <c r="BV17" s="57"/>
+      <c r="BR17" s="50"/>
+      <c r="BS17" s="50"/>
+      <c r="BT17" s="50"/>
+      <c r="BU17" s="50"/>
+      <c r="BV17" s="50"/>
       <c r="BW17" s="29"/>
     </row>
     <row r="18" spans="1:75" s="2" customFormat="1" x14ac:dyDescent="0.15">
@@ -5101,18 +5105,18 @@
       <c r="P18" s="33"/>
       <c r="Q18" s="33"/>
       <c r="R18" s="33"/>
-      <c r="S18" s="58" t="s">
+      <c r="S18" s="51" t="s">
         <v>45</v>
       </c>
-      <c r="T18" s="58"/>
-      <c r="U18" s="58"/>
-      <c r="V18" s="58"/>
-      <c r="W18" s="58"/>
-      <c r="X18" s="58"/>
-      <c r="Y18" s="58"/>
-      <c r="Z18" s="58"/>
-      <c r="AA18" s="58"/>
-      <c r="AB18" s="58"/>
+      <c r="T18" s="51"/>
+      <c r="U18" s="51"/>
+      <c r="V18" s="51"/>
+      <c r="W18" s="51"/>
+      <c r="X18" s="51"/>
+      <c r="Y18" s="51"/>
+      <c r="Z18" s="51"/>
+      <c r="AA18" s="51"/>
+      <c r="AB18" s="51"/>
       <c r="AC18" s="33"/>
       <c r="AD18" s="33"/>
       <c r="AE18" s="33"/>
@@ -5149,13 +5153,13 @@
       <c r="BJ18" s="33"/>
       <c r="BK18" s="33"/>
       <c r="BL18" s="33"/>
-      <c r="BM18" s="58" t="s">
+      <c r="BM18" s="51" t="s">
         <v>39</v>
       </c>
-      <c r="BN18" s="58"/>
-      <c r="BO18" s="58"/>
-      <c r="BP18" s="58"/>
-      <c r="BQ18" s="58"/>
+      <c r="BN18" s="51"/>
+      <c r="BO18" s="51"/>
+      <c r="BP18" s="51"/>
+      <c r="BQ18" s="51"/>
       <c r="BR18" s="33"/>
       <c r="BS18" s="33"/>
       <c r="BT18" s="33"/>
@@ -5178,24 +5182,24 @@
       <c r="L19" s="33"/>
       <c r="M19" s="33"/>
       <c r="N19" s="33"/>
-      <c r="O19" s="57" t="s">
+      <c r="O19" s="50" t="s">
         <v>38</v>
       </c>
-      <c r="P19" s="57"/>
-      <c r="Q19" s="57"/>
-      <c r="R19" s="57"/>
-      <c r="S19" s="57"/>
-      <c r="T19" s="57"/>
-      <c r="U19" s="57"/>
-      <c r="V19" s="57"/>
-      <c r="W19" s="57"/>
-      <c r="X19" s="57"/>
-      <c r="Y19" s="57"/>
-      <c r="Z19" s="57"/>
-      <c r="AA19" s="57"/>
-      <c r="AB19" s="57"/>
-      <c r="AC19" s="57"/>
-      <c r="AD19" s="57"/>
+      <c r="P19" s="50"/>
+      <c r="Q19" s="50"/>
+      <c r="R19" s="50"/>
+      <c r="S19" s="50"/>
+      <c r="T19" s="50"/>
+      <c r="U19" s="50"/>
+      <c r="V19" s="50"/>
+      <c r="W19" s="50"/>
+      <c r="X19" s="50"/>
+      <c r="Y19" s="50"/>
+      <c r="Z19" s="50"/>
+      <c r="AA19" s="50"/>
+      <c r="AB19" s="50"/>
+      <c r="AC19" s="50"/>
+      <c r="AD19" s="50"/>
       <c r="AE19" s="33"/>
       <c r="AF19" s="33"/>
       <c r="AG19" s="33"/>
@@ -5228,20 +5232,20 @@
       <c r="BH19" s="33"/>
       <c r="BI19" s="33"/>
       <c r="BJ19" s="33"/>
-      <c r="BK19" s="57" t="s">
+      <c r="BK19" s="50" t="s">
         <v>51</v>
       </c>
-      <c r="BL19" s="57"/>
-      <c r="BM19" s="57"/>
-      <c r="BN19" s="57"/>
-      <c r="BO19" s="57"/>
-      <c r="BP19" s="57"/>
-      <c r="BQ19" s="57"/>
-      <c r="BR19" s="57"/>
-      <c r="BS19" s="57"/>
-      <c r="BT19" s="57"/>
-      <c r="BU19" s="57"/>
-      <c r="BV19" s="57"/>
+      <c r="BL19" s="50"/>
+      <c r="BM19" s="50"/>
+      <c r="BN19" s="50"/>
+      <c r="BO19" s="50"/>
+      <c r="BP19" s="50"/>
+      <c r="BQ19" s="50"/>
+      <c r="BR19" s="50"/>
+      <c r="BS19" s="50"/>
+      <c r="BT19" s="50"/>
+      <c r="BU19" s="50"/>
+      <c r="BV19" s="50"/>
       <c r="BW19" s="29"/>
     </row>
     <row r="20" spans="1:75" s="2" customFormat="1" x14ac:dyDescent="0.15">
@@ -5256,20 +5260,20 @@
       <c r="I20" s="33"/>
       <c r="J20" s="33"/>
       <c r="K20" s="33"/>
-      <c r="L20" s="58" t="s">
+      <c r="L20" s="51" t="s">
         <v>44</v>
       </c>
-      <c r="M20" s="58"/>
-      <c r="N20" s="58"/>
-      <c r="O20" s="58"/>
-      <c r="P20" s="58"/>
-      <c r="Q20" s="58"/>
-      <c r="R20" s="58"/>
-      <c r="S20" s="58"/>
-      <c r="T20" s="58"/>
-      <c r="U20" s="58"/>
-      <c r="V20" s="58"/>
-      <c r="W20" s="58"/>
+      <c r="M20" s="51"/>
+      <c r="N20" s="51"/>
+      <c r="O20" s="51"/>
+      <c r="P20" s="51"/>
+      <c r="Q20" s="51"/>
+      <c r="R20" s="51"/>
+      <c r="S20" s="51"/>
+      <c r="T20" s="51"/>
+      <c r="U20" s="51"/>
+      <c r="V20" s="51"/>
+      <c r="W20" s="51"/>
       <c r="X20" s="33"/>
       <c r="Y20" s="33"/>
       <c r="Z20" s="33"/>
@@ -5300,25 +5304,25 @@
       <c r="AY20" s="33"/>
       <c r="AZ20" s="33"/>
       <c r="BA20" s="33"/>
-      <c r="BB20" s="58" t="s">
+      <c r="BB20" s="51" t="s">
         <v>49</v>
       </c>
-      <c r="BC20" s="58"/>
-      <c r="BD20" s="58"/>
-      <c r="BE20" s="58"/>
-      <c r="BF20" s="58"/>
-      <c r="BG20" s="58"/>
-      <c r="BH20" s="58"/>
-      <c r="BI20" s="58"/>
-      <c r="BJ20" s="58"/>
-      <c r="BK20" s="58"/>
-      <c r="BL20" s="58"/>
-      <c r="BM20" s="58"/>
-      <c r="BN20" s="58"/>
-      <c r="BO20" s="58"/>
-      <c r="BP20" s="58"/>
-      <c r="BQ20" s="58"/>
-      <c r="BR20" s="58"/>
+      <c r="BC20" s="51"/>
+      <c r="BD20" s="51"/>
+      <c r="BE20" s="51"/>
+      <c r="BF20" s="51"/>
+      <c r="BG20" s="51"/>
+      <c r="BH20" s="51"/>
+      <c r="BI20" s="51"/>
+      <c r="BJ20" s="51"/>
+      <c r="BK20" s="51"/>
+      <c r="BL20" s="51"/>
+      <c r="BM20" s="51"/>
+      <c r="BN20" s="51"/>
+      <c r="BO20" s="51"/>
+      <c r="BP20" s="51"/>
+      <c r="BQ20" s="51"/>
+      <c r="BR20" s="51"/>
       <c r="BS20" s="33"/>
       <c r="BT20" s="33"/>
       <c r="BU20" s="33"/>
@@ -5335,18 +5339,18 @@
       <c r="G21" s="33"/>
       <c r="H21" s="33"/>
       <c r="I21" s="33"/>
-      <c r="J21" s="57" t="s">
+      <c r="J21" s="50" t="s">
         <v>43</v>
       </c>
-      <c r="K21" s="57"/>
-      <c r="L21" s="57"/>
-      <c r="M21" s="57"/>
-      <c r="N21" s="57"/>
-      <c r="O21" s="57"/>
-      <c r="P21" s="57"/>
-      <c r="Q21" s="57"/>
-      <c r="R21" s="57"/>
-      <c r="S21" s="57"/>
+      <c r="K21" s="50"/>
+      <c r="L21" s="50"/>
+      <c r="M21" s="50"/>
+      <c r="N21" s="50"/>
+      <c r="O21" s="50"/>
+      <c r="P21" s="50"/>
+      <c r="Q21" s="50"/>
+      <c r="R21" s="50"/>
+      <c r="S21" s="50"/>
       <c r="T21" s="33"/>
       <c r="U21" s="33"/>
       <c r="V21" s="33"/>
@@ -5372,22 +5376,22 @@
       <c r="AP21" s="33"/>
       <c r="AQ21" s="33"/>
       <c r="AR21" s="33"/>
-      <c r="AS21" s="57" t="s">
+      <c r="AS21" s="50" t="s">
         <v>48</v>
       </c>
-      <c r="AT21" s="57"/>
-      <c r="AU21" s="57"/>
-      <c r="AV21" s="57"/>
-      <c r="AW21" s="57"/>
-      <c r="AX21" s="57"/>
-      <c r="AY21" s="57"/>
-      <c r="AZ21" s="57"/>
-      <c r="BA21" s="57"/>
-      <c r="BB21" s="57"/>
-      <c r="BC21" s="57"/>
-      <c r="BD21" s="57"/>
-      <c r="BE21" s="57"/>
-      <c r="BF21" s="57"/>
+      <c r="AT21" s="50"/>
+      <c r="AU21" s="50"/>
+      <c r="AV21" s="50"/>
+      <c r="AW21" s="50"/>
+      <c r="AX21" s="50"/>
+      <c r="AY21" s="50"/>
+      <c r="AZ21" s="50"/>
+      <c r="BA21" s="50"/>
+      <c r="BB21" s="50"/>
+      <c r="BC21" s="50"/>
+      <c r="BD21" s="50"/>
+      <c r="BE21" s="50"/>
+      <c r="BF21" s="50"/>
       <c r="BG21" s="33"/>
       <c r="BH21" s="33"/>
       <c r="BI21" s="33"/>
@@ -5414,13 +5418,13 @@
       <c r="E22" s="33"/>
       <c r="F22" s="33"/>
       <c r="G22" s="33"/>
-      <c r="H22" s="58" t="s">
+      <c r="H22" s="51" t="s">
         <v>5</v>
       </c>
-      <c r="I22" s="58"/>
-      <c r="J22" s="58"/>
-      <c r="K22" s="58"/>
-      <c r="L22" s="58"/>
+      <c r="I22" s="51"/>
+      <c r="J22" s="51"/>
+      <c r="K22" s="51"/>
+      <c r="L22" s="51"/>
       <c r="M22" s="33"/>
       <c r="N22" s="33"/>
       <c r="O22" s="33"/>
@@ -5442,21 +5446,21 @@
       <c r="AE22" s="33"/>
       <c r="AF22" s="33"/>
       <c r="AG22" s="33"/>
-      <c r="AH22" s="58" t="s">
+      <c r="AH22" s="51" t="s">
         <v>47</v>
       </c>
-      <c r="AI22" s="58"/>
-      <c r="AJ22" s="58"/>
-      <c r="AK22" s="58"/>
-      <c r="AL22" s="58"/>
-      <c r="AM22" s="58"/>
-      <c r="AN22" s="58"/>
-      <c r="AO22" s="58"/>
-      <c r="AP22" s="58"/>
-      <c r="AQ22" s="58"/>
-      <c r="AR22" s="58"/>
-      <c r="AS22" s="58"/>
-      <c r="AT22" s="58"/>
+      <c r="AI22" s="51"/>
+      <c r="AJ22" s="51"/>
+      <c r="AK22" s="51"/>
+      <c r="AL22" s="51"/>
+      <c r="AM22" s="51"/>
+      <c r="AN22" s="51"/>
+      <c r="AO22" s="51"/>
+      <c r="AP22" s="51"/>
+      <c r="AQ22" s="51"/>
+      <c r="AR22" s="51"/>
+      <c r="AS22" s="51"/>
+      <c r="AT22" s="51"/>
       <c r="AU22" s="33"/>
       <c r="AV22" s="33"/>
       <c r="AW22" s="33"/>
@@ -5490,14 +5494,14 @@
     <row r="23" spans="1:75" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A23" s="43"/>
       <c r="B23" s="33"/>
-      <c r="C23" s="57" t="s">
+      <c r="C23" s="50" t="s">
         <v>36</v>
       </c>
-      <c r="D23" s="57"/>
-      <c r="E23" s="57"/>
-      <c r="F23" s="57"/>
-      <c r="G23" s="57"/>
-      <c r="H23" s="57"/>
+      <c r="D23" s="50"/>
+      <c r="E23" s="50"/>
+      <c r="F23" s="50"/>
+      <c r="G23" s="50"/>
+      <c r="H23" s="50"/>
       <c r="I23" s="33"/>
       <c r="J23" s="33"/>
       <c r="K23" s="33"/>
@@ -5567,14 +5571,14 @@
       <c r="BW23" s="34"/>
     </row>
     <row r="24" spans="1:75" s="2" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A24" s="52" t="s">
+      <c r="A24" s="57" t="s">
         <v>37</v>
       </c>
-      <c r="B24" s="53"/>
-      <c r="C24" s="53"/>
-      <c r="D24" s="53"/>
-      <c r="E24" s="53"/>
-      <c r="F24" s="53"/>
+      <c r="B24" s="58"/>
+      <c r="C24" s="58"/>
+      <c r="D24" s="58"/>
+      <c r="E24" s="58"/>
+      <c r="F24" s="58"/>
       <c r="G24" s="33"/>
       <c r="H24" s="33"/>
       <c r="I24" s="33"/>
@@ -6297,107 +6301,107 @@
     <row r="30" spans="1:75" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A30" s="40"/>
       <c r="B30" s="25"/>
-      <c r="C30" s="50" t="s">
+      <c r="C30" s="48" t="s">
         <v>4</v>
       </c>
-      <c r="D30" s="50"/>
-      <c r="E30" s="50"/>
-      <c r="F30" s="50"/>
-      <c r="G30" s="50"/>
-      <c r="H30" s="50"/>
-      <c r="I30" s="56" t="s">
+      <c r="D30" s="48"/>
+      <c r="E30" s="48"/>
+      <c r="F30" s="48"/>
+      <c r="G30" s="48"/>
+      <c r="H30" s="48"/>
+      <c r="I30" s="49" t="s">
         <v>55</v>
       </c>
-      <c r="J30" s="56"/>
-      <c r="K30" s="56"/>
-      <c r="L30" s="56"/>
-      <c r="M30" s="56"/>
+      <c r="J30" s="49"/>
+      <c r="K30" s="49"/>
+      <c r="L30" s="49"/>
+      <c r="M30" s="49"/>
       <c r="N30" s="25"/>
       <c r="O30" s="25"/>
       <c r="P30" s="25"/>
       <c r="Q30" s="25"/>
-      <c r="R30" s="50" t="s">
+      <c r="R30" s="48" t="s">
         <v>56</v>
       </c>
-      <c r="S30" s="50"/>
-      <c r="T30" s="50"/>
-      <c r="U30" s="50"/>
-      <c r="V30" s="50"/>
-      <c r="W30" s="50"/>
-      <c r="X30" s="50"/>
+      <c r="S30" s="48"/>
+      <c r="T30" s="48"/>
+      <c r="U30" s="48"/>
+      <c r="V30" s="48"/>
+      <c r="W30" s="48"/>
+      <c r="X30" s="48"/>
       <c r="Y30" s="25"/>
       <c r="Z30" s="25"/>
-      <c r="AA30" s="48" t="s">
+      <c r="AA30" s="54" t="s">
         <v>52</v>
       </c>
-      <c r="AB30" s="48"/>
-      <c r="AC30" s="48"/>
+      <c r="AB30" s="54"/>
+      <c r="AC30" s="54"/>
       <c r="AD30" s="25"/>
       <c r="AE30" s="25"/>
       <c r="AF30" s="25"/>
       <c r="AG30" s="25"/>
       <c r="AH30" s="25"/>
-      <c r="AI30" s="51" t="s">
+      <c r="AI30" s="56" t="s">
         <v>57</v>
       </c>
-      <c r="AJ30" s="51"/>
-      <c r="AK30" s="51"/>
-      <c r="AL30" s="51"/>
-      <c r="AM30" s="51"/>
-      <c r="AN30" s="51"/>
-      <c r="AO30" s="51"/>
+      <c r="AJ30" s="56"/>
+      <c r="AK30" s="56"/>
+      <c r="AL30" s="56"/>
+      <c r="AM30" s="56"/>
+      <c r="AN30" s="56"/>
+      <c r="AO30" s="56"/>
       <c r="AP30" s="25"/>
       <c r="AQ30" s="25"/>
-      <c r="AR30" s="49" t="s">
+      <c r="AR30" s="55" t="s">
         <v>58</v>
       </c>
-      <c r="AS30" s="49"/>
-      <c r="AT30" s="49"/>
-      <c r="AU30" s="49"/>
-      <c r="AV30" s="49"/>
+      <c r="AS30" s="55"/>
+      <c r="AT30" s="55"/>
+      <c r="AU30" s="55"/>
+      <c r="AV30" s="55"/>
       <c r="AW30" s="25"/>
       <c r="AX30" s="25"/>
       <c r="AY30" s="25"/>
       <c r="AZ30" s="25"/>
-      <c r="BA30" s="50" t="s">
+      <c r="BA30" s="48" t="s">
         <v>59</v>
       </c>
-      <c r="BB30" s="50"/>
-      <c r="BC30" s="50"/>
-      <c r="BD30" s="50"/>
-      <c r="BE30" s="50"/>
-      <c r="BF30" s="50"/>
+      <c r="BB30" s="48"/>
+      <c r="BC30" s="48"/>
+      <c r="BD30" s="48"/>
+      <c r="BE30" s="48"/>
+      <c r="BF30" s="48"/>
       <c r="BG30" s="25"/>
-      <c r="BH30" s="49" t="s">
+      <c r="BH30" s="55" t="s">
         <v>53</v>
       </c>
-      <c r="BI30" s="49"/>
-      <c r="BJ30" s="49"/>
-      <c r="BK30" s="49"/>
-      <c r="BL30" s="49"/>
-      <c r="BM30" s="49"/>
-      <c r="BN30" s="49"/>
-      <c r="BO30" s="49"/>
+      <c r="BI30" s="55"/>
+      <c r="BJ30" s="55"/>
+      <c r="BK30" s="55"/>
+      <c r="BL30" s="55"/>
+      <c r="BM30" s="55"/>
+      <c r="BN30" s="55"/>
+      <c r="BO30" s="55"/>
       <c r="BP30" s="25"/>
-      <c r="BQ30" s="50" t="s">
+      <c r="BQ30" s="48" t="s">
         <v>54</v>
       </c>
-      <c r="BR30" s="50"/>
-      <c r="BS30" s="50"/>
-      <c r="BT30" s="50"/>
-      <c r="BU30" s="50"/>
-      <c r="BV30" s="50"/>
+      <c r="BR30" s="48"/>
+      <c r="BS30" s="48"/>
+      <c r="BT30" s="48"/>
+      <c r="BU30" s="48"/>
+      <c r="BV30" s="48"/>
       <c r="BW30" s="28"/>
     </row>
     <row r="31" spans="1:75" x14ac:dyDescent="0.15">
-      <c r="A31" s="54" t="s">
+      <c r="A31" s="46" t="s">
         <v>37</v>
       </c>
-      <c r="B31" s="55"/>
-      <c r="C31" s="55"/>
-      <c r="D31" s="55"/>
-      <c r="E31" s="55"/>
-      <c r="F31" s="55"/>
+      <c r="B31" s="47"/>
+      <c r="C31" s="47"/>
+      <c r="D31" s="47"/>
+      <c r="E31" s="47"/>
+      <c r="F31" s="47"/>
       <c r="G31" s="25"/>
       <c r="H31" s="25"/>
       <c r="I31" s="25"/>
@@ -6631,6 +6635,15 @@
     <row r="38" spans="1:75" s="20" customFormat="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <mergeCells count="25">
+    <mergeCell ref="A11:E11"/>
+    <mergeCell ref="AA30:AC30"/>
+    <mergeCell ref="AR30:AV30"/>
+    <mergeCell ref="BA30:BF30"/>
+    <mergeCell ref="BQ30:BV30"/>
+    <mergeCell ref="AI30:AO30"/>
+    <mergeCell ref="BH30:BO30"/>
+    <mergeCell ref="A24:F24"/>
+    <mergeCell ref="S18:AB18"/>
     <mergeCell ref="A31:F31"/>
     <mergeCell ref="C30:H30"/>
     <mergeCell ref="I30:M30"/>
@@ -6647,15 +6660,6 @@
     <mergeCell ref="J21:S21"/>
     <mergeCell ref="L20:W20"/>
     <mergeCell ref="O19:AD19"/>
-    <mergeCell ref="A11:E11"/>
-    <mergeCell ref="AA30:AC30"/>
-    <mergeCell ref="AR30:AV30"/>
-    <mergeCell ref="BA30:BF30"/>
-    <mergeCell ref="BQ30:BV30"/>
-    <mergeCell ref="AI30:AO30"/>
-    <mergeCell ref="BH30:BO30"/>
-    <mergeCell ref="A24:F24"/>
-    <mergeCell ref="S18:AB18"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>